<commit_message>
Reworked and retested some of the adapters
</commit_message>
<xml_diff>
--- a/adapterFPix2DTBTestProtocol_SN009.xlsx
+++ b/adapterFPix2DTBTestProtocol_SN009.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$79</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="67">
   <si>
     <t>FPix to DTB adapter v2.1 test protocol</t>
   </si>
@@ -171,18 +171,9 @@
     <t>Connect adapter (still with flex cable) to DTB. Issue power on command. LED should light up.</t>
   </si>
   <si>
-    <t>Connect adapter (still with flex cable) to DTB. Turn HV on.</t>
-  </si>
-  <si>
-    <t>Current rading after 20 s:</t>
-  </si>
-  <si>
     <t>Set Keithley voltage to -1000 V, current compliance 100 µA. Turn voltage on.</t>
   </si>
   <si>
-    <t>Keithley should not trip (ok within the first second)</t>
-  </si>
-  <si>
     <t>µA</t>
   </si>
   <si>
@@ -195,25 +186,53 @@
     <t>Frank Meier</t>
   </si>
   <si>
-    <t>4. Summary</t>
-  </si>
-  <si>
-    <t>Module test:</t>
-  </si>
-  <si>
     <t>Tester:</t>
   </si>
   <si>
     <t>Test date:</t>
+  </si>
+  <si>
+    <t>1) Do not connect the adapter. Turn HV on, read after 60 sec</t>
+  </si>
+  <si>
+    <t>2) Connect the adapter. Turn HV on, read after 60 sec</t>
+  </si>
+  <si>
+    <t>Keithley should not trip any time.</t>
+  </si>
+  <si>
+    <t>No adapter</t>
+  </si>
+  <si>
+    <t>With adapt.</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>4. Visual inspection</t>
+  </si>
+  <si>
+    <t>1) Jumper for LED installed</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>2) Kapton foil present on back side</t>
+  </si>
+  <si>
+    <t>3) S/N sticker attached</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd\-mmm\-yyyy"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -414,7 +433,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -448,8 +467,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="105">
@@ -889,10 +914,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I72"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -911,7 +936,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -1537,7 +1562,7 @@
         <v>90.9</v>
       </c>
       <c r="F34" s="5" t="str">
-        <f>IF(ABS(E34-C34)&lt;=D34,"ok","NOK")</f>
+        <f t="shared" ref="F34:F40" si="2">IF(ABS(E34-C34)&lt;=D34,"ok","NOK")</f>
         <v>ok</v>
       </c>
       <c r="L34">
@@ -1563,7 +1588,7 @@
         <v>120.6</v>
       </c>
       <c r="F35" s="5" t="str">
-        <f>IF(ABS(E35-C35)&lt;=D35,"ok","NOK")</f>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
       <c r="L35">
@@ -1589,7 +1614,7 @@
         <v>120.4</v>
       </c>
       <c r="F36" s="5" t="str">
-        <f>IF(ABS(E36-C36)&lt;=D36,"ok","NOK")</f>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
       <c r="L36">
@@ -1616,7 +1641,7 @@
         <v>168.9</v>
       </c>
       <c r="F37" s="5" t="str">
-        <f>IF(ABS(E37-C37)&lt;=D37,"ok","NOK")</f>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
       <c r="L37">
@@ -1643,7 +1668,7 @@
         <v>168.8</v>
       </c>
       <c r="F38" s="5" t="str">
-        <f>IF(ABS(E38-C38)&lt;=D38,"ok","NOK")</f>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
       <c r="L38">
@@ -1670,7 +1695,7 @@
         <v>168.7</v>
       </c>
       <c r="F39" s="5" t="str">
-        <f>IF(ABS(E39-C39)&lt;=D39,"ok","NOK")</f>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
       <c r="L39">
@@ -1696,7 +1721,7 @@
         <v>30</v>
       </c>
       <c r="F40" s="5" t="str">
-        <f>IF(ABS(E40-C40)&lt;=D40,"ok","NOK")</f>
+        <f t="shared" si="2"/>
         <v>ok</v>
       </c>
       <c r="L40">
@@ -1890,62 +1915,126 @@
     </row>
     <row r="60" spans="1:4">
       <c r="B60" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="B61" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="B62" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="B64" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="16">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D63" s="4" t="s">
+    </row>
+    <row r="65" spans="1:7">
+      <c r="B65" t="s">
+        <v>60</v>
+      </c>
+      <c r="C65" s="16">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="B66" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" s="16">
+        <f>C65-C64</f>
+        <v>1.9000000000000003E-2</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F66" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="C67" s="16"/>
+      <c r="D67" s="4"/>
+      <c r="G67" s="17"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="14" t="str">
+        <f>IF(C66&lt;=F66,"PASS","FAIL")</f>
+        <v>FAIL</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="18">
+      <c r="A71" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" s="14"/>
+      <c r="D73" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>65</v>
+      </c>
+      <c r="B74" s="14"/>
+      <c r="D74" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>66</v>
+      </c>
+      <c r="B75" s="14"/>
+      <c r="D75" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="B76" s="14"/>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="B77" s="14"/>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>54</v>
+      </c>
+      <c r="B79" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" t="s">
-        <v>54</v>
-      </c>
-      <c r="C64" s="5">
-        <v>0.01</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" t="s">
-        <v>43</v>
-      </c>
-      <c r="B66" s="14"/>
-    </row>
-    <row r="68" spans="1:6" ht="18">
-      <c r="A68" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
-        <v>58</v>
-      </c>
-      <c r="B70" s="14"/>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" t="s">
-        <v>56</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F72" s="15">
-        <v>41829</v>
+      <c r="E79" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F79" s="15">
+        <v>41830</v>
       </c>
     </row>
   </sheetData>

</xml_diff>